<commit_message>
updated readme and sample
</commit_message>
<xml_diff>
--- a/extras/sample_form/slider_sample.xlsx
+++ b/extras/sample_form/slider_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\slider\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF4BFDD-27BB-4F62-AFAB-26373ABD0C58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DA127B-6AB1-49C2-9743-54352A226895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="383">
   <si>
     <t>type</t>
   </si>
@@ -2981,9 +2983,6 @@
   </si>
   <si>
     <t>Range field-list</t>
-  </si>
-  <si>
-    <t>custom-slider(min="1",max="150")</t>
   </si>
   <si>
     <t>results_note</t>
@@ -3000,7 +2999,16 @@
     <t>Slider 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Slider 1  </t>
+    <t>custom-slider(min="1",max="10")</t>
+  </si>
+  <si>
+    <t>.&gt;4</t>
+  </si>
+  <si>
+    <t>Slide higher</t>
+  </si>
+  <si>
+    <t>Slider 1 with Consraint</t>
   </si>
 </sst>
 </file>
@@ -3343,7 +3351,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="288">
+  <dxfs count="237">
     <dxf>
       <fill>
         <patternFill>
@@ -4255,131 +4263,131 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAC090"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB9CDE5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7E4BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4BD97"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3D69B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB3A2C7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9CDE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7E4BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4BD97"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB3A2C7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9E004F"/>
+          <bgColor rgb="FFBFBFBF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4389,16 +4397,6 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF6D9E"/>
         </patternFill>
       </fill>
@@ -4406,6 +4404,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFF2DBDA"/>
         </patternFill>
       </fill>
@@ -4420,7 +4425,21 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF6969"/>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7D480"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4428,389 +4447,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFEBF1DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCD5B5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9CDE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7E4BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4BD97"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB3A2C7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCC1DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEBF1DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCE6F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCD5B5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB9CDE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7E4BD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4BD97"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB3A2C7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFB00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5823,7 +5459,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -6066,13 +5702,19 @@
         <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>375</v>
+        <v>379</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -6097,13 +5739,13 @@
         <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="L14" s="3"/>
     </row>
@@ -6115,13 +5757,13 @@
         <v>372</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="L15" s="3"/>
     </row>
@@ -6138,603 +5780,420 @@
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I11 F1:F11 B15 B1:C14 I13:I14 F13:F14 F16:F1048576 I16:I1048576 B16:C1048576">
-    <cfRule type="expression" dxfId="287" priority="361">
+  <conditionalFormatting sqref="B15 B1:C14 F16:F1048576 I16:I1048576 B16:C1048576 I1:I14 F1:F14">
+    <cfRule type="expression" dxfId="236" priority="361">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O11 I1:I11 B15 B1:C14 O13:O14 I13:I14 I16:I1048576 O16:O1048576 B16:C1048576">
-    <cfRule type="expression" dxfId="286" priority="362">
+  <conditionalFormatting sqref="B15 B1:C14 I16:I1048576 O16:O1048576 B16:C1048576 I1:I14 O1:O14">
+    <cfRule type="expression" dxfId="235" priority="362">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 F1:F11 B1:D11 F13:F14 B13:D14 B16:D1048576 F16:F1048576">
-    <cfRule type="expression" dxfId="285" priority="363">
+  <conditionalFormatting sqref="B15 B16:D1048576 F16:F1048576 B1:D14 F1:F14">
+    <cfRule type="expression" dxfId="234" priority="363">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 G1:H11 B1:D11 G13:H14 B13:D14 L14 B16:D1048576 G16:H1048576">
-    <cfRule type="expression" dxfId="284" priority="364">
+  <conditionalFormatting sqref="B15 L14 B16:D1048576 G16:H1048576 B1:D14 G1:H14">
+    <cfRule type="expression" dxfId="233" priority="364">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 G1:H11 B1:D11 G13:H14 B13:D14 L14 B16:D1048576 G16:H1048576">
-    <cfRule type="expression" dxfId="283" priority="365">
+  <conditionalFormatting sqref="B15 L14 B16:D1048576 G16:H1048576 B1:D14 G1:H14">
+    <cfRule type="expression" dxfId="232" priority="365">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 B15 B1:C14 F13:F14 F16:F1048576 B16:C1048576">
-    <cfRule type="expression" dxfId="282" priority="366">
+  <conditionalFormatting sqref="B15 B1:C14 F16:F1048576 B16:C1048576 F1:F14">
+    <cfRule type="expression" dxfId="231" priority="366">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 F13:F14 F16:F1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="281" priority="367">
+  <conditionalFormatting sqref="F16:F1048576 B1:B1048576 F1:F14">
+    <cfRule type="expression" dxfId="230" priority="367">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 B1:C14 B16:C1048576">
-    <cfRule type="expression" dxfId="280" priority="368">
+    <cfRule type="expression" dxfId="229" priority="368">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="279" priority="369">
+    <cfRule type="expression" dxfId="228" priority="369">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="370">
+    <cfRule type="expression" dxfId="227" priority="370">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N11 N13:N14 N16:N1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="277" priority="371">
+  <conditionalFormatting sqref="N16:N1048576 B1:B1048576 N1:N14">
+    <cfRule type="expression" dxfId="226" priority="371">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 B15 B1:C14 F13:F14 F16:F1048576 B16:C1048576">
-    <cfRule type="expression" dxfId="276" priority="372">
+  <conditionalFormatting sqref="B15 B1:C14 F16:F1048576 B16:C1048576 F1:F14">
+    <cfRule type="expression" dxfId="225" priority="372">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 B15 B1:C14 F13:F14 F16:F1048576 B16:C1048576">
-    <cfRule type="expression" dxfId="275" priority="373">
+  <conditionalFormatting sqref="B15 B1:C14 F16:F1048576 B16:C1048576 F1:F14">
+    <cfRule type="expression" dxfId="224" priority="373">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 B1:C14 B16:C1048576">
-    <cfRule type="expression" dxfId="274" priority="374">
+    <cfRule type="expression" dxfId="223" priority="374">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15 A1:W11 A13:W14 A16:W1048576">
-    <cfRule type="expression" dxfId="273" priority="375">
+  <conditionalFormatting sqref="B15 A16:W1048576 A1:W14">
+    <cfRule type="expression" dxfId="222" priority="375">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="376">
+    <cfRule type="expression" dxfId="221" priority="376">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="271" priority="377">
+    <cfRule type="expression" dxfId="220" priority="377">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="378">
+    <cfRule type="expression" dxfId="219" priority="378">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="379">
+    <cfRule type="expression" dxfId="218" priority="379">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="380">
+    <cfRule type="expression" dxfId="217" priority="380">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="381">
+    <cfRule type="expression" dxfId="216" priority="381">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="266" priority="382">
+    <cfRule type="expression" dxfId="215" priority="382">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="265" priority="383">
+    <cfRule type="expression" dxfId="214" priority="383">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="384">
+    <cfRule type="expression" dxfId="213" priority="384">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="263" priority="385">
+    <cfRule type="expression" dxfId="212" priority="385">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="386">
+    <cfRule type="expression" dxfId="211" priority="386">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="261" priority="387">
+    <cfRule type="expression" dxfId="210" priority="387">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="260" priority="388">
+    <cfRule type="expression" dxfId="209" priority="388">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="259" priority="389">
+    <cfRule type="expression" dxfId="208" priority="389">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="390">
+    <cfRule type="expression" dxfId="207" priority="390">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="257" priority="391">
+    <cfRule type="expression" dxfId="206" priority="391">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="392">
+    <cfRule type="expression" dxfId="205" priority="392">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="393">
+    <cfRule type="expression" dxfId="204" priority="393">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="254" priority="394">
+    <cfRule type="expression" dxfId="203" priority="394">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F11 F13:F14 F16:F1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="253" priority="395">
+  <conditionalFormatting sqref="F16:F1048576 B1:B1048576 F1:F14">
+    <cfRule type="expression" dxfId="202" priority="395">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="expression" dxfId="252" priority="191">
+    <cfRule type="expression" dxfId="201" priority="191">
       <formula>$A15="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15 I15">
-    <cfRule type="expression" dxfId="251" priority="192">
+    <cfRule type="expression" dxfId="200" priority="192">
       <formula>$A15="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="250" priority="193">
+    <cfRule type="expression" dxfId="199" priority="193">
       <formula>$A15="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:H15 D15">
-    <cfRule type="expression" dxfId="249" priority="194">
+    <cfRule type="expression" dxfId="198" priority="194">
       <formula>$A15="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:H15 D15">
-    <cfRule type="expression" dxfId="248" priority="195">
+    <cfRule type="expression" dxfId="197" priority="195">
       <formula>$A15="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="expression" dxfId="247" priority="201">
+    <cfRule type="expression" dxfId="196" priority="201">
       <formula>OR($A15="calculate", $A15="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15 D15:E15 M15:W15 G15:K15">
-    <cfRule type="expression" dxfId="246" priority="205">
+    <cfRule type="expression" dxfId="195" priority="205">
       <formula>OR(AND(LEFT($A15, 14)="sensor_stream ", LEN($A15)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A15, 15)))), AND(LEFT($A15, 17)="sensor_statistic ", LEN($A15)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A15, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="245" priority="206">
+    <cfRule type="expression" dxfId="194" priority="206">
       <formula>$A15="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="207">
+    <cfRule type="expression" dxfId="193" priority="207">
       <formula>OR($A15="audio", $A15="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="208">
+    <cfRule type="expression" dxfId="192" priority="208">
       <formula>$A15="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="209">
+    <cfRule type="expression" dxfId="191" priority="209">
       <formula>OR($A15="date", $A15="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="210">
+    <cfRule type="expression" dxfId="190" priority="210">
       <formula>OR($A15="calculate", $A15="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="211">
+    <cfRule type="expression" dxfId="189" priority="211">
       <formula>$A15="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="239" priority="212">
+    <cfRule type="expression" dxfId="188" priority="212">
       <formula>$A15="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="213">
+    <cfRule type="expression" dxfId="187" priority="213">
       <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="214">
+    <cfRule type="expression" dxfId="186" priority="214">
       <formula>OR($A15="audio audit", $A15="text audit", $A15="speed violations count", $A15="speed violations list", $A15="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="215">
+    <cfRule type="expression" dxfId="185" priority="215">
       <formula>OR($A15="username", $A15="phonenumber", $A15="start", $A15="end", $A15="deviceid", $A15="subscriberid", $A15="simserial", $A15="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="216">
+    <cfRule type="expression" dxfId="184" priority="216">
       <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="217">
+    <cfRule type="expression" dxfId="183" priority="217">
       <formula>$A15="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="218">
+    <cfRule type="expression" dxfId="182" priority="218">
       <formula>$A15="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="219">
+    <cfRule type="expression" dxfId="181" priority="219">
       <formula>$A15="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="220">
+    <cfRule type="expression" dxfId="180" priority="220">
       <formula>$A15="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="230" priority="221">
+    <cfRule type="expression" dxfId="179" priority="221">
       <formula>$A15="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="222">
+    <cfRule type="expression" dxfId="178" priority="222">
       <formula>$A15="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="223">
+    <cfRule type="expression" dxfId="177" priority="223">
       <formula>$A15="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="expression" dxfId="227" priority="170">
+    <cfRule type="expression" dxfId="176" priority="170">
       <formula>$A15="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="expression" dxfId="226" priority="171">
+    <cfRule type="expression" dxfId="175" priority="171">
       <formula>$A15="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="expression" dxfId="225" priority="172">
+    <cfRule type="expression" dxfId="174" priority="172">
       <formula>OR(AND(LEFT($A15, 14)="sensor_stream ", LEN($A15)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A15, 15)))), AND(LEFT($A15, 17)="sensor_statistic ", LEN($A15)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A15, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="173">
+    <cfRule type="expression" dxfId="173" priority="173">
       <formula>$A15="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="174">
+    <cfRule type="expression" dxfId="172" priority="174">
       <formula>OR($A15="audio", $A15="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="175">
+    <cfRule type="expression" dxfId="171" priority="175">
       <formula>$A15="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="176">
+    <cfRule type="expression" dxfId="170" priority="176">
       <formula>OR($A15="date", $A15="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="177">
+    <cfRule type="expression" dxfId="169" priority="177">
       <formula>OR($A15="calculate", $A15="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="178">
+    <cfRule type="expression" dxfId="168" priority="178">
       <formula>$A15="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="179">
+    <cfRule type="expression" dxfId="167" priority="179">
       <formula>$A15="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="180">
+    <cfRule type="expression" dxfId="166" priority="180">
       <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="181">
+    <cfRule type="expression" dxfId="165" priority="181">
       <formula>OR($A15="audio audit", $A15="text audit", $A15="speed violations count", $A15="speed violations list", $A15="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="215" priority="182">
+    <cfRule type="expression" dxfId="164" priority="182">
       <formula>OR($A15="username", $A15="phonenumber", $A15="start", $A15="end", $A15="deviceid", $A15="subscriberid", $A15="simserial", $A15="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="183">
+    <cfRule type="expression" dxfId="163" priority="183">
       <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="184">
+    <cfRule type="expression" dxfId="162" priority="184">
       <formula>$A15="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="185">
+    <cfRule type="expression" dxfId="161" priority="185">
       <formula>$A15="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="186">
+    <cfRule type="expression" dxfId="160" priority="186">
       <formula>$A15="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="187">
+    <cfRule type="expression" dxfId="159" priority="187">
       <formula>$A15="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="188">
+    <cfRule type="expression" dxfId="158" priority="188">
       <formula>$A15="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="189">
+    <cfRule type="expression" dxfId="157" priority="189">
       <formula>$A15="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="207" priority="190">
+    <cfRule type="expression" dxfId="156" priority="190">
       <formula>$A15="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="expression" dxfId="206" priority="135">
-      <formula>$A12="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12 O12">
-    <cfRule type="expression" dxfId="205" priority="136">
-      <formula>$A12="begin repeat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:D12">
-    <cfRule type="expression" dxfId="204" priority="137">
-      <formula>$A12="text"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:D12 G12:H12">
-    <cfRule type="expression" dxfId="203" priority="138">
-      <formula>$A12="integer"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:D12 G12:H12">
-    <cfRule type="expression" dxfId="202" priority="139">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N12">
-    <cfRule type="expression" dxfId="201" priority="145">
-      <formula>OR($A12="calculate", $A12="calculate_here")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12:E12 G12:W12">
-    <cfRule type="expression" dxfId="200" priority="149">
-      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="199" priority="150">
-      <formula>$A12="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="198" priority="151">
-      <formula>OR($A12="audio", $A12="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="197" priority="152">
-      <formula>$A12="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="196" priority="153">
-      <formula>OR($A12="date", $A12="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="195" priority="154">
-      <formula>OR($A12="calculate", $A12="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="194" priority="155">
-      <formula>$A12="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="193" priority="156">
-      <formula>$A12="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="192" priority="157">
-      <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="191" priority="158">
-      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="190" priority="159">
-      <formula>OR($A12="username", $A12="phonenumber", $A12="start", $A12="end", $A12="deviceid", $A12="subscriberid", $A12="simserial", $A12="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="189" priority="160">
-      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="188" priority="161">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="187" priority="162">
-      <formula>$A12="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="186" priority="163">
-      <formula>$A12="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="185" priority="164">
-      <formula>$A12="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="184" priority="165">
-      <formula>$A12="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="166">
-      <formula>$A12="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="182" priority="167">
-      <formula>$A12="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="181" priority="53">
+    <cfRule type="expression" dxfId="155" priority="53">
       <formula>$A15="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="180" priority="54">
+    <cfRule type="expression" dxfId="154" priority="54">
       <formula>$A15="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="179" priority="55">
+    <cfRule type="expression" dxfId="153" priority="55">
       <formula>$A15="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="178" priority="56">
+    <cfRule type="expression" dxfId="152" priority="56">
       <formula>$A15="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="177" priority="57">
+    <cfRule type="expression" dxfId="151" priority="57">
       <formula>$A15="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="176" priority="58">
+    <cfRule type="expression" dxfId="150" priority="58">
       <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="175" priority="59">
+    <cfRule type="expression" dxfId="149" priority="59">
       <formula>$A15="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="60">
+    <cfRule type="expression" dxfId="148" priority="60">
       <formula>$A15="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="61">
+    <cfRule type="expression" dxfId="147" priority="61">
       <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="172" priority="62">
+    <cfRule type="expression" dxfId="146" priority="62">
       <formula>OR($A15="date", $A15="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="171" priority="63">
+    <cfRule type="expression" dxfId="145" priority="63">
       <formula>$A15="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="170" priority="64">
+    <cfRule type="expression" dxfId="144" priority="64">
       <formula>OR($A15="audio", $A15="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="169" priority="65">
+    <cfRule type="expression" dxfId="143" priority="65">
       <formula>OR(AND(LEFT($A15, 14)="sensor_stream ", LEN($A15)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A15, 15)))), AND(LEFT($A15, 17)="sensor_statistic ", LEN($A15)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A15, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="66">
+    <cfRule type="expression" dxfId="142" priority="66">
       <formula>$A15="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="67">
+    <cfRule type="expression" dxfId="141" priority="67">
       <formula>OR($A15="audio", $A15="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="68">
+    <cfRule type="expression" dxfId="140" priority="68">
       <formula>$A15="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="69">
+    <cfRule type="expression" dxfId="139" priority="69">
       <formula>OR($A15="date", $A15="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="70">
+    <cfRule type="expression" dxfId="138" priority="70">
       <formula>OR($A15="calculate", $A15="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="71">
+    <cfRule type="expression" dxfId="137" priority="71">
       <formula>$A15="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="72">
+    <cfRule type="expression" dxfId="136" priority="72">
       <formula>$A15="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="73">
+    <cfRule type="expression" dxfId="135" priority="73">
       <formula>OR($A15="geopoint", $A15="geoshape", $A15="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="74">
+    <cfRule type="expression" dxfId="134" priority="74">
       <formula>OR($A15="audio audit", $A15="text audit", $A15="speed violations count", $A15="speed violations list", $A15="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="75">
+    <cfRule type="expression" dxfId="133" priority="75">
       <formula>OR($A15="username", $A15="phonenumber", $A15="start", $A15="end", $A15="deviceid", $A15="subscriberid", $A15="simserial", $A15="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="76">
+    <cfRule type="expression" dxfId="132" priority="76">
       <formula>OR(AND(LEFT($A15, 16)="select_multiple ", LEN($A15)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A15, 17)))), AND(LEFT($A15, 11)="select_one ", LEN($A15)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A15, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="77">
+    <cfRule type="expression" dxfId="131" priority="77">
       <formula>$A15="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="78">
+    <cfRule type="expression" dxfId="130" priority="78">
       <formula>$A15="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="79">
+    <cfRule type="expression" dxfId="129" priority="79">
       <formula>$A15="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="80">
+    <cfRule type="expression" dxfId="128" priority="80">
       <formula>$A15="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="81">
+    <cfRule type="expression" dxfId="127" priority="81">
       <formula>$A15="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="82">
+    <cfRule type="expression" dxfId="126" priority="82">
       <formula>$A15="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="83">
+    <cfRule type="expression" dxfId="125" priority="83">
       <formula>$A15="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="150" priority="27">
-      <formula>$A12="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="149" priority="28">
-      <formula>$A12="text"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="148" priority="29">
-      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="147" priority="30">
-      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="146" priority="31">
-      <formula>OR($A12="date", $A12="datetime")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="145" priority="32">
-      <formula>$A12="image"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="144" priority="33">
-      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="143" priority="34">
-      <formula>$A12="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="35">
-      <formula>OR($A12="audio", $A12="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="36">
-      <formula>$A12="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="37">
-      <formula>OR($A12="date", $A12="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="38">
-      <formula>OR($A12="calculate", $A12="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="39">
-      <formula>$A12="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="40">
-      <formula>$A12="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="41">
-      <formula>OR($A12="geopoint", $A12="geoshape", $A12="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="42">
-      <formula>OR($A12="audio audit", $A12="text audit", $A12="speed violations count", $A12="speed violations list", $A12="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="43">
-      <formula>OR($A12="username", $A12="phonenumber", $A12="start", $A12="end", $A12="deviceid", $A12="subscriberid", $A12="simserial", $A12="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="44">
-      <formula>OR(AND(LEFT($A12, 16)="select_multiple ", LEN($A12)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A12, 17)))), AND(LEFT($A12, 11)="select_one ", LEN($A12)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A12, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="132" priority="45">
-      <formula>$A12="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="131" priority="46">
-      <formula>$A12="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="47">
-      <formula>$A12="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="48">
-      <formula>$A12="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="128" priority="49">
-      <formula>$A12="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="50">
-      <formula>$A12="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="51">
-      <formula>$A12="begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="125" priority="52">
-      <formula>OR(AND(LEFT($A12, 14)="sensor_stream ", LEN($A12)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A12, 15)))), AND(LEFT($A12, 17)="sensor_statistic ", LEN($A12)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A12, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
@@ -6951,7 +6410,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003111425</v>
+        <v>2003161821</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
@@ -7088,7 +6547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="19" customFormat="1" ht="202.8">
+    <row r="6" spans="1:30" s="19" customFormat="1" ht="187.2">
       <c r="A6" s="18" t="s">
         <v>77</v>
       </c>
@@ -7406,7 +6865,7 @@
       <c r="AC14" s="23"/>
       <c r="AD14" s="23"/>
     </row>
-    <row r="15" spans="1:30" s="25" customFormat="1" ht="46.8">
+    <row r="15" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A15" s="23" t="s">
         <v>116</v>
       </c>
@@ -7486,7 +6945,7 @@
       <c r="AC16" s="23"/>
       <c r="AD16" s="23"/>
     </row>
-    <row r="17" spans="1:30" s="25" customFormat="1" ht="62.4">
+    <row r="17" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A17" s="23" t="s">
         <v>116</v>
       </c>
@@ -7606,7 +7065,7 @@
       <c r="AC19" s="23"/>
       <c r="AD19" s="23"/>
     </row>
-    <row r="20" spans="1:30" s="25" customFormat="1" ht="46.8">
+    <row r="20" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A20" s="23" t="s">
         <v>116</v>
       </c>
@@ -11277,7 +10736,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" s="19" customFormat="1" ht="312">
+    <row r="6" spans="1:8" s="19" customFormat="1" ht="296.39999999999998">
       <c r="A6" s="18" t="s">
         <v>366</v>
       </c>

</xml_diff>

<commit_message>
added processing of decimals
</commit_message>
<xml_diff>
--- a/extras/sample_form/slider_sample.xlsx
+++ b/extras/sample_form/slider_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\slider\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DA127B-6AB1-49C2-9743-54352A226895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CA5492-C530-4C43-9DDC-AE465DFF5B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="385">
   <si>
     <t>type</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>integer</t>
-  </si>
-  <si>
-    <t>This is the hint text.</t>
   </si>
   <si>
     <t>begin group</t>
@@ -2999,16 +2996,25 @@
     <t>Slider 3</t>
   </si>
   <si>
-    <t>custom-slider(min="1",max="10")</t>
-  </si>
-  <si>
-    <t>.&gt;4</t>
-  </si>
-  <si>
-    <t>Slide higher</t>
-  </si>
-  <si>
-    <t>Slider 1 with Consraint</t>
+    <t>custom-slider(min="0",max="1.5")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slider 1 </t>
+  </si>
+  <si>
+    <t>Slider Range 0 - 10</t>
+  </si>
+  <si>
+    <t>Slider Range 0 - 1000</t>
+  </si>
+  <si>
+    <t>Slider Range 0 - 1.5</t>
+  </si>
+  <si>
+    <t>custom-slider(min="0",max="10")</t>
+  </si>
+  <si>
+    <t>custom-slider(min="0",max="1000")</t>
   </si>
 </sst>
 </file>
@@ -5456,10 +5462,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -5699,36 +5705,30 @@
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>380</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -5736,43 +5736,43 @@
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>381</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:27">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="46.8">
@@ -5780,10 +5780,10 @@
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -6315,41 +6315,41 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -6382,40 +6382,40 @@
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>64</v>
       </c>
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003161821</v>
+        <v>2003171216</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
       <c r="F2" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -6441,7 +6441,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1">
       <c r="A1" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="42"/>
     </row>
@@ -6451,7 +6451,7 @@
     </row>
     <row r="3" spans="1:30" ht="97" customHeight="1">
       <c r="A3" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="44"/>
     </row>
@@ -6466,13 +6466,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>4</v>
@@ -6487,7 +6487,7 @@
         <v>7</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>8</v>
@@ -6502,7 +6502,7 @@
         <v>11</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="5" t="s">
         <v>12</v>
@@ -6523,13 +6523,13 @@
         <v>21</v>
       </c>
       <c r="W5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="Y5" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>22</v>
@@ -6549,99 +6549,99 @@
     </row>
     <row r="6" spans="1:30" s="19" customFormat="1" ht="187.2">
       <c r="A6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="I6" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="K6" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="L6" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="M6" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="N6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="O6" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="P6" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="P6" s="18" t="s">
+      <c r="Q6" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="R6" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="S6" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="T6" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="T6" s="18" t="s">
+      <c r="U6" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="U6" s="18" t="s">
+      <c r="V6" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="V6" s="18" t="s">
+      <c r="W6" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="W6" s="18" t="s">
+      <c r="X6" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="X6" s="18" t="s">
+      <c r="Y6" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="Y6" s="18" t="s">
+      <c r="Z6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="Z6" s="18" t="s">
+      <c r="AA6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="AA6" s="18" t="s">
+      <c r="AB6" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="AB6" s="18" t="s">
+      <c r="AC6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="AC6" s="18" t="s">
+      <c r="AD6" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="AD6" s="18" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:30" s="22" customFormat="1">
       <c r="A8" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="45"/>
       <c r="C8" s="20"/>
@@ -6675,13 +6675,13 @@
     </row>
     <row r="10" spans="1:30" s="25" customFormat="1">
       <c r="A10" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="C10" s="24" t="s">
         <v>109</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>110</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -6713,20 +6713,20 @@
     </row>
     <row r="11" spans="1:30" s="25" customFormat="1">
       <c r="A11" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>109</v>
-      </c>
       <c r="C11" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
@@ -6756,10 +6756,10 @@
         <v>43</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -6791,13 +6791,13 @@
     </row>
     <row r="13" spans="1:30" s="25" customFormat="1">
       <c r="A13" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>115</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -6829,13 +6829,13 @@
     </row>
     <row r="14" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A14" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>116</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>117</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -6867,20 +6867,20 @@
     </row>
     <row r="15" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A15" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
       <c r="H15" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
@@ -6907,20 +6907,20 @@
     </row>
     <row r="16" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A16" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
       <c r="H16" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
@@ -6947,20 +6947,20 @@
     </row>
     <row r="17" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A17" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
       <c r="H17" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
@@ -6987,20 +6987,20 @@
     </row>
     <row r="18" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A18" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
@@ -7027,20 +7027,20 @@
     </row>
     <row r="19" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A19" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I19" s="23"/>
       <c r="J19" s="23"/>
@@ -7067,20 +7067,20 @@
     </row>
     <row r="20" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A20" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
@@ -7107,20 +7107,20 @@
     </row>
     <row r="21" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A21" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I21" s="23"/>
       <c r="J21" s="23"/>
@@ -7147,20 +7147,20 @@
     </row>
     <row r="22" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A22" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
@@ -7187,20 +7187,20 @@
     </row>
     <row r="23" spans="1:30" s="25" customFormat="1" ht="78">
       <c r="A23" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
       <c r="H23" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I23" s="23"/>
       <c r="J23" s="23"/>
@@ -7227,20 +7227,20 @@
     </row>
     <row r="24" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A24" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
@@ -7267,20 +7267,20 @@
     </row>
     <row r="25" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A25" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
@@ -7307,20 +7307,20 @@
     </row>
     <row r="26" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A26" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
       <c r="H26" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
@@ -7347,20 +7347,20 @@
     </row>
     <row r="27" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A27" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I27" s="23"/>
       <c r="J27" s="23"/>
@@ -7387,20 +7387,20 @@
     </row>
     <row r="28" spans="1:30" s="25" customFormat="1" ht="78">
       <c r="A28" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
       <c r="H28" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I28" s="23"/>
       <c r="J28" s="23"/>
@@ -7427,13 +7427,13 @@
     </row>
     <row r="29" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A29" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="24" t="s">
         <v>146</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>147</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
@@ -7465,20 +7465,20 @@
     </row>
     <row r="30" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A30" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
       <c r="G30" s="23"/>
       <c r="H30" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I30" s="23"/>
       <c r="J30" s="23"/>
@@ -7505,20 +7505,20 @@
     </row>
     <row r="31" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A31" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
       <c r="H31" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I31" s="23"/>
       <c r="J31" s="23"/>
@@ -7545,20 +7545,20 @@
     </row>
     <row r="32" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A32" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
       <c r="H32" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I32" s="23"/>
       <c r="J32" s="23"/>
@@ -7585,20 +7585,20 @@
     </row>
     <row r="33" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A33" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
       <c r="H33" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I33" s="23"/>
       <c r="J33" s="23"/>
@@ -7625,20 +7625,20 @@
     </row>
     <row r="34" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A34" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
       <c r="H34" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I34" s="23"/>
       <c r="J34" s="23"/>
@@ -7665,20 +7665,20 @@
     </row>
     <row r="35" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A35" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I35" s="23"/>
       <c r="J35" s="23"/>
@@ -7705,20 +7705,20 @@
     </row>
     <row r="36" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A36" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>
       <c r="H36" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I36" s="23"/>
       <c r="J36" s="23"/>
@@ -7745,20 +7745,20 @@
     </row>
     <row r="37" spans="1:30" s="25" customFormat="1" ht="78">
       <c r="A37" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="23"/>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
       <c r="H37" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I37" s="23"/>
       <c r="J37" s="23"/>
@@ -7785,13 +7785,13 @@
     </row>
     <row r="38" spans="1:30" s="25" customFormat="1">
       <c r="A38" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="24" t="s">
         <v>156</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>157</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="23"/>
@@ -7823,13 +7823,13 @@
     </row>
     <row r="39" spans="1:30" s="25" customFormat="1">
       <c r="A39" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="24" t="s">
         <v>158</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>159</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="23"/>
@@ -7861,13 +7861,13 @@
     </row>
     <row r="40" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A40" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>160</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>161</v>
       </c>
       <c r="D40" s="23"/>
       <c r="E40" s="23"/>
@@ -7899,13 +7899,13 @@
     </row>
     <row r="41" spans="1:30" s="25" customFormat="1">
       <c r="A41" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="24" t="s">
         <v>162</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>163</v>
       </c>
       <c r="D41" s="23"/>
       <c r="E41" s="23"/>
@@ -7937,13 +7937,13 @@
     </row>
     <row r="42" spans="1:30" s="25" customFormat="1">
       <c r="A42" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
@@ -7975,20 +7975,20 @@
     </row>
     <row r="43" spans="1:30" s="25" customFormat="1">
       <c r="A43" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D43" s="23"/>
       <c r="E43" s="23"/>
       <c r="F43" s="23"/>
       <c r="G43" s="23"/>
       <c r="H43" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I43" s="23"/>
       <c r="J43" s="23"/>
@@ -8015,13 +8015,13 @@
     </row>
     <row r="44" spans="1:30" s="25" customFormat="1">
       <c r="A44" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="24" t="s">
         <v>168</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>169</v>
       </c>
       <c r="D44" s="23"/>
       <c r="E44" s="23"/>
@@ -8053,20 +8053,20 @@
     </row>
     <row r="45" spans="1:30" s="25" customFormat="1">
       <c r="A45" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D45" s="23"/>
       <c r="E45" s="23"/>
       <c r="F45" s="23"/>
       <c r="G45" s="23"/>
       <c r="H45" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -8093,13 +8093,13 @@
     </row>
     <row r="46" spans="1:30" s="25" customFormat="1">
       <c r="A46" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C46" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D46" s="23"/>
       <c r="E46" s="23"/>
@@ -8131,20 +8131,20 @@
     </row>
     <row r="47" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A47" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D47" s="23"/>
       <c r="E47" s="23"/>
       <c r="F47" s="23"/>
       <c r="G47" s="23"/>
       <c r="H47" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I47" s="23"/>
       <c r="J47" s="23"/>
@@ -8171,20 +8171,20 @@
     </row>
     <row r="48" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A48" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D48" s="23"/>
       <c r="E48" s="23"/>
       <c r="F48" s="23"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="23"/>
@@ -8211,20 +8211,20 @@
     </row>
     <row r="49" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A49" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="23"/>
       <c r="F49" s="23"/>
       <c r="G49" s="23"/>
       <c r="H49" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I49" s="23"/>
       <c r="J49" s="23"/>
@@ -8251,13 +8251,13 @@
     </row>
     <row r="50" spans="1:30" s="25" customFormat="1">
       <c r="A50" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="24" t="s">
         <v>178</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>179</v>
       </c>
       <c r="D50" s="23"/>
       <c r="E50" s="23"/>
@@ -8289,13 +8289,13 @@
     </row>
     <row r="51" spans="1:30" s="25" customFormat="1">
       <c r="A51" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="24" t="s">
         <v>180</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>181</v>
       </c>
       <c r="D51" s="23"/>
       <c r="E51" s="23"/>
@@ -8327,13 +8327,13 @@
     </row>
     <row r="52" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A52" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="24" t="s">
         <v>182</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>183</v>
       </c>
       <c r="D52" s="23"/>
       <c r="E52" s="23"/>
@@ -8368,10 +8368,10 @@
         <v>23</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D53" s="23"/>
       <c r="E53" s="23"/>
@@ -8406,7 +8406,7 @@
         <v>27</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="23"/>
@@ -8442,7 +8442,7 @@
         <v>30</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C55" s="24"/>
       <c r="D55" s="23"/>
@@ -8478,7 +8478,7 @@
         <v>32</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56" s="23"/>
@@ -8514,7 +8514,7 @@
         <v>33</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="23"/>
@@ -8550,7 +8550,7 @@
         <v>34</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C58" s="24"/>
       <c r="D58" s="23"/>
@@ -8586,7 +8586,7 @@
         <v>42</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C59" s="24"/>
       <c r="D59" s="23"/>
@@ -8622,7 +8622,7 @@
         <v>36</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C60" s="24"/>
       <c r="D60" s="23"/>
@@ -8655,10 +8655,10 @@
     </row>
     <row r="61" spans="1:30" s="25" customFormat="1">
       <c r="A61" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C61" s="24"/>
       <c r="D61" s="23"/>
@@ -8694,7 +8694,7 @@
         <v>39</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C62" s="24"/>
       <c r="D62" s="23"/>
@@ -8712,7 +8712,7 @@
       <c r="P62" s="23"/>
       <c r="Q62" s="23"/>
       <c r="R62" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S62" s="23"/>
       <c r="T62" s="23"/>
@@ -8729,10 +8729,10 @@
     </row>
     <row r="63" spans="1:30" s="25" customFormat="1">
       <c r="A63" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C63" s="24"/>
       <c r="D63" s="23"/>
@@ -8750,7 +8750,7 @@
       <c r="P63" s="23"/>
       <c r="Q63" s="23"/>
       <c r="R63" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S63" s="23"/>
       <c r="T63" s="23"/>
@@ -8767,10 +8767,10 @@
     </row>
     <row r="64" spans="1:30" s="25" customFormat="1">
       <c r="A64" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" s="24"/>
       <c r="D64" s="23"/>
@@ -8778,7 +8778,7 @@
       <c r="F64" s="23"/>
       <c r="G64" s="23"/>
       <c r="H64" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I64" s="23"/>
       <c r="J64" s="23"/>
@@ -8805,10 +8805,10 @@
     </row>
     <row r="65" spans="1:30" s="25" customFormat="1">
       <c r="A65" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C65" s="24"/>
       <c r="D65" s="23"/>
@@ -8816,7 +8816,7 @@
       <c r="F65" s="23"/>
       <c r="G65" s="23"/>
       <c r="H65" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I65" s="23"/>
       <c r="J65" s="23"/>
@@ -8843,10 +8843,10 @@
     </row>
     <row r="66" spans="1:30" s="25" customFormat="1">
       <c r="A66" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C66" s="24"/>
       <c r="D66" s="23"/>
@@ -8854,7 +8854,7 @@
       <c r="F66" s="23"/>
       <c r="G66" s="23"/>
       <c r="H66" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I66" s="23"/>
       <c r="J66" s="23"/>
@@ -8881,10 +8881,10 @@
     </row>
     <row r="67" spans="1:30" s="25" customFormat="1">
       <c r="A67" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67" s="23"/>
@@ -8892,7 +8892,7 @@
       <c r="F67" s="23"/>
       <c r="G67" s="23"/>
       <c r="H67" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I67" s="23"/>
       <c r="J67" s="23"/>
@@ -8919,13 +8919,13 @@
     </row>
     <row r="68" spans="1:30" s="25" customFormat="1">
       <c r="A68" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B68" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C68" s="24" t="s">
         <v>195</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>196</v>
       </c>
       <c r="D68" s="23"/>
       <c r="E68" s="23"/>
@@ -8957,7 +8957,7 @@
     </row>
     <row r="69" spans="1:30" s="25" customFormat="1">
       <c r="A69" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B69" s="23"/>
       <c r="C69" s="24"/>
@@ -8991,10 +8991,10 @@
     </row>
     <row r="70" spans="1:30" s="25" customFormat="1">
       <c r="A70" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C70" s="24"/>
       <c r="D70" s="23"/>
@@ -9027,13 +9027,13 @@
     </row>
     <row r="71" spans="1:30" s="25" customFormat="1">
       <c r="A71" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="B71" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="B71" s="23" t="s">
+      <c r="C71" s="24" t="s">
         <v>199</v>
-      </c>
-      <c r="C71" s="24" t="s">
-        <v>200</v>
       </c>
       <c r="D71" s="23"/>
       <c r="E71" s="23"/>
@@ -9065,7 +9065,7 @@
     </row>
     <row r="72" spans="1:30" s="25" customFormat="1">
       <c r="A72" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B72" s="23"/>
       <c r="C72" s="24"/>
@@ -9099,10 +9099,10 @@
     </row>
     <row r="73" spans="1:30" s="25" customFormat="1">
       <c r="A73" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C73" s="24"/>
       <c r="D73" s="23"/>
@@ -9135,13 +9135,13 @@
     </row>
     <row r="74" spans="1:30" s="25" customFormat="1">
       <c r="A74" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="B74" s="23" t="s">
-        <v>199</v>
-      </c>
       <c r="C74" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D74" s="23"/>
       <c r="E74" s="23"/>
@@ -9175,7 +9175,7 @@
     </row>
     <row r="75" spans="1:30" s="25" customFormat="1">
       <c r="A75" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="24"/>
@@ -9209,10 +9209,10 @@
     </row>
     <row r="76" spans="1:30" s="25" customFormat="1">
       <c r="A76" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C76" s="24"/>
       <c r="D76" s="23"/>
@@ -9245,10 +9245,10 @@
     </row>
     <row r="77" spans="1:30" s="25" customFormat="1">
       <c r="A77" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C77" s="24"/>
       <c r="D77" s="23"/>
@@ -9281,10 +9281,10 @@
     </row>
     <row r="78" spans="1:30" s="25" customFormat="1">
       <c r="A78" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C78" s="24"/>
       <c r="D78" s="23"/>
@@ -9317,10 +9317,10 @@
     </row>
     <row r="79" spans="1:30" s="25" customFormat="1">
       <c r="A79" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C79" s="24"/>
       <c r="D79" s="23"/>
@@ -9328,7 +9328,7 @@
       <c r="F79" s="23"/>
       <c r="G79" s="23"/>
       <c r="H79" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I79" s="23"/>
       <c r="J79" s="23"/>
@@ -9355,10 +9355,10 @@
     </row>
     <row r="80" spans="1:30" s="25" customFormat="1">
       <c r="A80" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C80" s="24"/>
       <c r="D80" s="23"/>
@@ -9366,7 +9366,7 @@
       <c r="F80" s="23"/>
       <c r="G80" s="23"/>
       <c r="H80" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I80" s="23"/>
       <c r="J80" s="23"/>
@@ -9393,10 +9393,10 @@
     </row>
     <row r="81" spans="1:30" s="25" customFormat="1">
       <c r="A81" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C81" s="24"/>
       <c r="D81" s="23"/>
@@ -9404,7 +9404,7 @@
       <c r="F81" s="23"/>
       <c r="G81" s="23"/>
       <c r="H81" s="23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I81" s="23"/>
       <c r="J81" s="23"/>
@@ -9431,7 +9431,7 @@
     </row>
     <row r="83" spans="1:30">
       <c r="A83" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B83" s="46"/>
       <c r="C83" s="28"/>
@@ -9465,27 +9465,27 @@
     </row>
     <row r="85" spans="1:30">
       <c r="A85" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="B85" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="B85" s="31" t="s">
+      <c r="C85" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="C85" s="31" t="s">
+      <c r="D85" s="31" t="s">
         <v>214</v>
-      </c>
-      <c r="D85" s="31" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="86" spans="1:30">
       <c r="A86" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B86" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="B86" s="32" t="s">
+      <c r="C86" s="32" t="s">
         <v>217</v>
-      </c>
-      <c r="C86" s="32" t="s">
-        <v>218</v>
       </c>
       <c r="D86" s="32">
         <v>2</v>
@@ -9493,10 +9493,10 @@
     </row>
     <row r="87" spans="1:30">
       <c r="A87" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B87" s="32" t="s">
         <v>219</v>
-      </c>
-      <c r="B87" s="32" t="s">
-        <v>220</v>
       </c>
       <c r="C87" s="33" t="str">
         <f>"3 - 2"</f>
@@ -9508,13 +9508,13 @@
     </row>
     <row r="88" spans="1:30">
       <c r="A88" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="B88" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="B88" s="32" t="s">
+      <c r="C88" s="32" t="s">
         <v>222</v>
-      </c>
-      <c r="C88" s="32" t="s">
-        <v>223</v>
       </c>
       <c r="D88" s="32">
         <v>6</v>
@@ -9522,13 +9522,13 @@
     </row>
     <row r="89" spans="1:30">
       <c r="A89" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B89" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="B89" s="32" t="s">
+      <c r="C89" s="32" t="s">
         <v>225</v>
-      </c>
-      <c r="C89" s="32" t="s">
-        <v>226</v>
       </c>
       <c r="D89" s="32">
         <v>5</v>
@@ -9536,13 +9536,13 @@
     </row>
     <row r="90" spans="1:30">
       <c r="A90" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B90" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="B90" s="32" t="s">
+      <c r="C90" s="32" t="s">
         <v>228</v>
-      </c>
-      <c r="C90" s="32" t="s">
-        <v>229</v>
       </c>
       <c r="D90" s="32">
         <v>1</v>
@@ -9550,128 +9550,128 @@
     </row>
     <row r="91" spans="1:30">
       <c r="A91" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B91" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="B91" s="32" t="s">
+      <c r="C91" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="C91" s="32" t="s">
+      <c r="D91" s="32" t="s">
         <v>232</v>
-      </c>
-      <c r="D91" s="32" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="92" spans="1:30">
       <c r="A92" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B92" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="B92" s="32" t="s">
+      <c r="C92" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="C92" s="32" t="s">
-        <v>236</v>
-      </c>
       <c r="D92" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="93" spans="1:30">
       <c r="A93" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B93" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="B93" s="32" t="s">
+      <c r="C93" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="C93" s="32" t="s">
-        <v>239</v>
-      </c>
       <c r="D93" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:30">
       <c r="A94" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="B94" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="B94" s="32" t="s">
+      <c r="C94" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="C94" s="32" t="s">
-        <v>242</v>
-      </c>
       <c r="D94" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:30">
       <c r="A95" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="B95" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="B95" s="32" t="s">
+      <c r="C95" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="C95" s="32" t="s">
-        <v>245</v>
-      </c>
       <c r="D95" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="96" spans="1:30">
       <c r="A96" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B96" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="B96" s="32" t="s">
+      <c r="C96" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="C96" s="32" t="s">
-        <v>248</v>
-      </c>
       <c r="D96" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B97" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="B97" s="32" t="s">
+      <c r="C97" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="C97" s="32" t="s">
-        <v>251</v>
-      </c>
       <c r="D97" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="B98" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="B98" s="32" t="s">
+      <c r="C98" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="C98" s="32" t="s">
-        <v>254</v>
-      </c>
       <c r="D98" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="B99" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="B99" s="32" t="s">
+      <c r="C99" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="C99" s="32" t="s">
+      <c r="D99" s="32" t="s">
         <v>257</v>
-      </c>
-      <c r="D99" s="32" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -9683,330 +9683,330 @@
     <row r="101" spans="1:4">
       <c r="A101" s="29"/>
       <c r="B101" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D101" s="29"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="29"/>
       <c r="B102" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C102" s="35" t="s">
         <v>260</v>
-      </c>
-      <c r="C102" s="35" t="s">
-        <v>261</v>
       </c>
       <c r="D102" s="29"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="29"/>
       <c r="B103" s="35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C103" s="35" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D103" s="29"/>
     </row>
     <row r="104" spans="1:4" ht="31.2">
       <c r="A104" s="29"/>
       <c r="B104" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="C104" s="35" t="s">
         <v>262</v>
-      </c>
-      <c r="C104" s="35" t="s">
-        <v>263</v>
       </c>
       <c r="D104" s="29"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="29"/>
       <c r="B105" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="C105" s="35" t="s">
         <v>264</v>
-      </c>
-      <c r="C105" s="35" t="s">
-        <v>265</v>
       </c>
       <c r="D105" s="29"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="29"/>
       <c r="B106" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="C106" s="35" t="s">
         <v>266</v>
-      </c>
-      <c r="C106" s="35" t="s">
-        <v>267</v>
       </c>
       <c r="D106" s="29"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="29"/>
       <c r="B107" s="35" t="s">
+        <v>267</v>
+      </c>
+      <c r="C107" s="35" t="s">
         <v>268</v>
-      </c>
-      <c r="C107" s="35" t="s">
-        <v>269</v>
       </c>
       <c r="D107" s="29"/>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="29"/>
       <c r="B108" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="C108" s="35" t="s">
         <v>270</v>
-      </c>
-      <c r="C108" s="35" t="s">
-        <v>271</v>
       </c>
       <c r="D108" s="29"/>
     </row>
     <row r="109" spans="1:4" ht="46.8">
       <c r="A109" s="29"/>
       <c r="B109" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="C109" s="35" t="s">
         <v>272</v>
-      </c>
-      <c r="C109" s="35" t="s">
-        <v>273</v>
       </c>
       <c r="D109" s="29"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="29"/>
       <c r="B110" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="C110" s="35" t="s">
         <v>274</v>
-      </c>
-      <c r="C110" s="35" t="s">
-        <v>275</v>
       </c>
       <c r="D110" s="29"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="29"/>
       <c r="B111" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C111" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D111" s="29"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="29"/>
       <c r="B112" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="C112" s="35" t="s">
         <v>277</v>
-      </c>
-      <c r="C112" s="35" t="s">
-        <v>278</v>
       </c>
       <c r="D112" s="29"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="29"/>
       <c r="B113" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="C113" s="35" t="s">
         <v>279</v>
-      </c>
-      <c r="C113" s="35" t="s">
-        <v>280</v>
       </c>
       <c r="D113" s="29"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="29"/>
       <c r="B114" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="C114" s="35" t="s">
         <v>281</v>
-      </c>
-      <c r="C114" s="35" t="s">
-        <v>282</v>
       </c>
       <c r="D114" s="29"/>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="29"/>
       <c r="B115" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="C115" s="35" t="s">
         <v>283</v>
-      </c>
-      <c r="C115" s="35" t="s">
-        <v>284</v>
       </c>
       <c r="D115" s="29"/>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="29"/>
       <c r="B116" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="C116" s="35" t="s">
         <v>285</v>
-      </c>
-      <c r="C116" s="35" t="s">
-        <v>286</v>
       </c>
       <c r="D116" s="29"/>
     </row>
     <row r="117" spans="1:4" ht="31.2">
       <c r="A117" s="29"/>
       <c r="B117" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="C117" s="35" t="s">
         <v>287</v>
-      </c>
-      <c r="C117" s="35" t="s">
-        <v>288</v>
       </c>
       <c r="D117" s="29"/>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="29"/>
       <c r="B118" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="C118" s="35" t="s">
         <v>289</v>
-      </c>
-      <c r="C118" s="35" t="s">
-        <v>290</v>
       </c>
       <c r="D118" s="29"/>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="29"/>
       <c r="B119" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="C119" s="35" t="s">
         <v>291</v>
-      </c>
-      <c r="C119" s="35" t="s">
-        <v>292</v>
       </c>
       <c r="D119" s="29"/>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="29"/>
       <c r="B120" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="C120" s="35" t="s">
         <v>293</v>
-      </c>
-      <c r="C120" s="35" t="s">
-        <v>294</v>
       </c>
       <c r="D120" s="29"/>
     </row>
     <row r="121" spans="1:4" ht="31.2">
       <c r="A121" s="29"/>
       <c r="B121" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="C121" s="35" t="s">
         <v>295</v>
-      </c>
-      <c r="C121" s="35" t="s">
-        <v>296</v>
       </c>
       <c r="D121" s="29"/>
     </row>
     <row r="122" spans="1:4" ht="46.8">
       <c r="A122" s="29"/>
       <c r="B122" s="35" t="s">
+        <v>296</v>
+      </c>
+      <c r="C122" s="35" t="s">
         <v>297</v>
-      </c>
-      <c r="C122" s="35" t="s">
-        <v>298</v>
       </c>
       <c r="D122" s="29"/>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="29"/>
       <c r="B123" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="C123" s="35" t="s">
         <v>299</v>
-      </c>
-      <c r="C123" s="35" t="s">
-        <v>300</v>
       </c>
       <c r="D123" s="29"/>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="29"/>
       <c r="B124" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="C124" s="35" t="s">
         <v>301</v>
-      </c>
-      <c r="C124" s="35" t="s">
-        <v>302</v>
       </c>
       <c r="D124" s="29"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="29"/>
       <c r="B125" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="C125" s="35" t="s">
         <v>303</v>
-      </c>
-      <c r="C125" s="35" t="s">
-        <v>304</v>
       </c>
       <c r="D125" s="29"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="29"/>
       <c r="B126" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="C126" s="35" t="s">
         <v>305</v>
-      </c>
-      <c r="C126" s="35" t="s">
-        <v>306</v>
       </c>
       <c r="D126" s="29"/>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="29"/>
       <c r="B127" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="C127" s="35" t="s">
         <v>307</v>
-      </c>
-      <c r="C127" s="35" t="s">
-        <v>308</v>
       </c>
       <c r="D127" s="29"/>
     </row>
     <row r="128" spans="1:4" ht="31.2">
       <c r="A128" s="29"/>
       <c r="B128" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="C128" s="35" t="s">
         <v>309</v>
-      </c>
-      <c r="C128" s="35" t="s">
-        <v>310</v>
       </c>
       <c r="D128" s="29"/>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="29"/>
       <c r="B129" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="C129" s="36" t="s">
         <v>311</v>
-      </c>
-      <c r="C129" s="36" t="s">
-        <v>312</v>
       </c>
       <c r="D129" s="29"/>
     </row>
     <row r="130" spans="1:4" ht="31.2">
       <c r="A130" s="29"/>
       <c r="B130" s="36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C130" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D130" s="29"/>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="29"/>
       <c r="B131" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C131" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D131" s="29"/>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="29"/>
       <c r="B132" s="36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C132" s="36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D132" s="29"/>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="29"/>
       <c r="B133" s="36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C133" s="36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D133" s="29"/>
     </row>
@@ -10023,200 +10023,200 @@
     <row r="135" spans="1:4">
       <c r="A135" s="29"/>
       <c r="B135" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="C135" s="36" t="s">
         <v>317</v>
-      </c>
-      <c r="C135" s="36" t="s">
-        <v>318</v>
       </c>
       <c r="D135" s="29"/>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="29"/>
       <c r="B136" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C136" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D136" s="29"/>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="29"/>
       <c r="B137" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="C137" s="36" t="s">
         <v>320</v>
-      </c>
-      <c r="C137" s="36" t="s">
-        <v>321</v>
       </c>
       <c r="D137" s="29"/>
     </row>
     <row r="138" spans="1:4" ht="31.2">
       <c r="A138" s="29"/>
       <c r="B138" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="C138" s="36" t="s">
         <v>322</v>
-      </c>
-      <c r="C138" s="36" t="s">
-        <v>323</v>
       </c>
       <c r="D138" s="29"/>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="29"/>
       <c r="B139" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="C139" s="36" t="s">
         <v>324</v>
-      </c>
-      <c r="C139" s="36" t="s">
-        <v>325</v>
       </c>
       <c r="D139" s="29"/>
     </row>
     <row r="140" spans="1:4" ht="31.2">
       <c r="A140" s="29"/>
       <c r="B140" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="C140" s="36" t="s">
         <v>326</v>
-      </c>
-      <c r="C140" s="36" t="s">
-        <v>327</v>
       </c>
       <c r="D140" s="29"/>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="29"/>
       <c r="B141" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="C141" s="36" t="s">
         <v>328</v>
-      </c>
-      <c r="C141" s="36" t="s">
-        <v>329</v>
       </c>
       <c r="D141" s="29"/>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="29"/>
       <c r="B142" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="C142" s="36" t="s">
         <v>330</v>
-      </c>
-      <c r="C142" s="36" t="s">
-        <v>331</v>
       </c>
       <c r="D142" s="29"/>
     </row>
     <row r="143" spans="1:4" ht="31.2">
       <c r="A143" s="29"/>
       <c r="B143" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="C143" s="36" t="s">
         <v>332</v>
-      </c>
-      <c r="C143" s="36" t="s">
-        <v>333</v>
       </c>
       <c r="D143" s="29"/>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="29"/>
       <c r="B144" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="C144" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="C144" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="D144" s="29"/>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="29"/>
       <c r="B145" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="C145" s="36" t="s">
         <v>336</v>
-      </c>
-      <c r="C145" s="36" t="s">
-        <v>337</v>
       </c>
       <c r="D145" s="29"/>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="29"/>
       <c r="B146" s="36" t="s">
+        <v>337</v>
+      </c>
+      <c r="C146" s="36" t="s">
         <v>338</v>
-      </c>
-      <c r="C146" s="36" t="s">
-        <v>339</v>
       </c>
       <c r="D146" s="29"/>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="29"/>
       <c r="B147" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="C147" s="36" t="s">
         <v>340</v>
-      </c>
-      <c r="C147" s="36" t="s">
-        <v>341</v>
       </c>
       <c r="D147" s="29"/>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="29"/>
       <c r="B148" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="C148" s="36" t="s">
         <v>342</v>
-      </c>
-      <c r="C148" s="36" t="s">
-        <v>343</v>
       </c>
       <c r="D148" s="29"/>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="29"/>
       <c r="B149" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="C149" s="36" t="s">
         <v>344</v>
-      </c>
-      <c r="C149" s="36" t="s">
-        <v>345</v>
       </c>
       <c r="D149" s="29"/>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="29"/>
       <c r="B150" s="36" t="s">
+        <v>345</v>
+      </c>
+      <c r="C150" s="36" t="s">
         <v>346</v>
-      </c>
-      <c r="C150" s="36" t="s">
-        <v>347</v>
       </c>
       <c r="D150" s="29"/>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="29"/>
       <c r="B151" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="C151" s="36" t="s">
         <v>348</v>
-      </c>
-      <c r="C151" s="36" t="s">
-        <v>349</v>
       </c>
       <c r="D151" s="29"/>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="29"/>
       <c r="B152" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="C152" s="36" t="s">
         <v>350</v>
-      </c>
-      <c r="C152" s="36" t="s">
-        <v>351</v>
       </c>
       <c r="D152" s="29"/>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="29"/>
       <c r="B153" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="C153" s="36" t="s">
         <v>352</v>
-      </c>
-      <c r="C153" s="36" t="s">
-        <v>353</v>
       </c>
       <c r="D153" s="29"/>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="29"/>
       <c r="B154" s="36" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C154" s="36" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D154" s="29"/>
     </row>
@@ -10594,7 +10594,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B1" s="42"/>
     </row>
@@ -10604,54 +10604,54 @@
     </row>
     <row r="3" spans="1:8" ht="99" customHeight="1">
       <c r="A3" s="44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B3" s="44"/>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="19" customFormat="1" ht="202.8">
       <c r="A6" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
         <v>359</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>362</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>363</v>
       </c>
       <c r="H6" s="18"/>
     </row>
@@ -10681,7 +10681,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16" customHeight="1">
       <c r="A1" s="47" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="38"/>
@@ -10699,7 +10699,7 @@
     </row>
     <row r="3" spans="1:8" ht="55" customHeight="1">
       <c r="A3" s="44" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="38"/>
@@ -10717,43 +10717,43 @@
     </row>
     <row r="5" spans="1:8" s="5" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="C5" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="D5" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="E5" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="F5" s="40" t="s">
         <v>63</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>64</v>
       </c>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" s="19" customFormat="1" ht="296.39999999999998">
       <c r="A6" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>368</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>370</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:8">

</xml_diff>

<commit_message>
display value and fit slider thumb properly
</commit_message>
<xml_diff>
--- a/extras/sample_form/slider_sample.xlsx
+++ b/extras/sample_form/slider_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\slider\extras\sample_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CA5492-C530-4C43-9DDC-AE465DFF5B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF07EA1-E6A4-4353-816C-CDAB57904970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2996,25 +2996,25 @@
     <t>Slider 3</t>
   </si>
   <si>
-    <t>custom-slider(min="0",max="1.5")</t>
-  </si>
-  <si>
     <t xml:space="preserve">Slider 1 </t>
   </si>
   <si>
-    <t>Slider Range 0 - 10</t>
-  </si>
-  <si>
-    <t>Slider Range 0 - 1000</t>
-  </si>
-  <si>
-    <t>Slider Range 0 - 1.5</t>
-  </si>
-  <si>
-    <t>custom-slider(min="0",max="10")</t>
-  </si>
-  <si>
-    <t>custom-slider(min="0",max="1000")</t>
+    <t>custom-slider(min="0",max="20", step=2, display_value="yes")</t>
+  </si>
+  <si>
+    <t>custom-slider(min="0",max="1", step=0.01, display_value="yes")</t>
+  </si>
+  <si>
+    <t>Slider Range 0 - 100</t>
+  </si>
+  <si>
+    <t>custom-slider(min="0",max="100", step=1)</t>
+  </si>
+  <si>
+    <t>Slider Range 0 - 20</t>
+  </si>
+  <si>
+    <t>Slider Range 0 - 1</t>
   </si>
 </sst>
 </file>
@@ -5462,10 +5462,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -5708,13 +5708,13 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -5745,7 +5745,7 @@
         <v>381</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L14" s="3"/>
     </row>
@@ -5760,10 +5760,10 @@
         <v>377</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="L15" s="3"/>
     </row>
@@ -6410,7 +6410,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003171216</v>
+        <v>2003241520</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>

</xml_diff>